<commit_message>
ENH: Update newlife with relative reference
</commit_message>
<xml_diff>
--- a/lifelib/projects/newlife/model/Input/input.xlsx
+++ b/lifelib/projects/newlife/model/Input/input.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="6" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12940" windowWidth="24930" xWindow="80" yWindow="80"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="80" yWindow="80" windowWidth="24930" windowHeight="12940" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="PolicyData" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Mortality" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="ProductSpec" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="OtherParams" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Assumption" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="AssumptionTables" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Scenarios" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PolicyData" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mortality" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ProductSpec" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OtherParams" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Assumption" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssumptionTables" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Scenarios" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="AsmpByDuration">AssumptionTables!$B$7:$J$27</definedName>
@@ -31,10 +31,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt formatCode="0.000000_ " numFmtId="164"/>
-    <numFmt formatCode="0.0%" numFmtId="165"/>
-    <numFmt formatCode="0.0000" numFmtId="166"/>
-    <numFmt formatCode="0.0000%" numFmtId="167"/>
+    <numFmt numFmtId="164" formatCode="0.000000_ "/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -218,148 +218,148 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="38">
+    <xf numFmtId="38" fontId="1" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="9">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="44">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="4" fillId="2" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="5" fillId="2" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="2" numFmtId="9" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="2" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="10" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="2" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="10" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="6" numFmtId="9" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="38" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="38" fontId="4" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="2" numFmtId="9" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="2" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="6" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="2" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="2" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="2" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="3" fillId="2" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="2" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="6" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="2" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="2" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="0" name="標準" xfId="0"/>
-    <cellStyle builtinId="6" name="桁区切り" xfId="1"/>
-    <cellStyle builtinId="5" name="パーセント" xfId="2"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="桁区切り" xfId="1" builtinId="6"/>
+    <cellStyle name="パーセント" xfId="2" builtinId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -656,29 +656,29 @@
   </sheetPr>
   <dimension ref="B7:P307"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:O307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="1" width="20.7265625"/>
-    <col customWidth="1" max="2" min="2" style="1" width="10.36328125"/>
-    <col customWidth="1" max="3" min="3" style="1" width="11.7265625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="1" width="11.6328125"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="1" width="5.36328125"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="1" width="8.81640625"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="1" width="9"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="1" width="5"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="1" width="10.26953125"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="1" width="14.81640625"/>
-    <col customWidth="1" max="11" min="11" style="1" width="13.81640625"/>
-    <col bestFit="1" customWidth="1" max="12" min="12" style="1" width="11.81640625"/>
-    <col bestFit="1" customWidth="1" max="13" min="13" style="1" width="15.81640625"/>
-    <col bestFit="1" customWidth="1" max="14" min="14" style="1" width="12.36328125"/>
-    <col bestFit="1" customWidth="1" max="15" min="15" style="1" width="13.453125"/>
-    <col customWidth="1" max="16" min="16" style="1" width="9"/>
-    <col customWidth="1" max="16384" min="17" style="1" width="9"/>
+    <col width="20.7265625" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="10.36328125" customWidth="1" style="1" min="2" max="2"/>
+    <col width="11.7265625" customWidth="1" style="1" min="3" max="3"/>
+    <col width="11.6328125" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
+    <col width="5.36328125" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
+    <col width="8.81640625" bestFit="1" customWidth="1" style="1" min="6" max="6"/>
+    <col width="9" bestFit="1" customWidth="1" style="1" min="7" max="7"/>
+    <col width="5" bestFit="1" customWidth="1" style="1" min="8" max="8"/>
+    <col width="10.26953125" bestFit="1" customWidth="1" style="1" min="9" max="9"/>
+    <col width="14.81640625" bestFit="1" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.81640625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="11.81640625" bestFit="1" customWidth="1" style="1" min="12" max="12"/>
+    <col width="15.81640625" bestFit="1" customWidth="1" style="1" min="13" max="13"/>
+    <col width="12.36328125" bestFit="1" customWidth="1" style="1" min="14" max="14"/>
+    <col width="13.453125" bestFit="1" customWidth="1" style="1" min="15" max="15"/>
+    <col width="9" customWidth="1" style="1" min="16" max="16"/>
+    <col width="9" customWidth="1" style="1" min="17" max="16384"/>
   </cols>
   <sheetData>
     <row r="7">
@@ -14755,7 +14755,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
@@ -14768,280 +14768,280 @@
   </sheetPr>
   <dimension ref="B1:Q137"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.08984375" defaultRowHeight="12.5"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="4" width="6.7265625"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="4" width="9.6328125"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="4" width="26.7265625"/>
-    <col customWidth="1" max="4" min="4" style="4" width="8.7265625"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="4" width="9.6328125"/>
-    <col customWidth="1" max="13" min="6" style="4" width="10.6328125"/>
-    <col customWidth="1" max="247" min="14" style="4" width="9.08984375"/>
-    <col customWidth="1" max="249" min="248" style="4" width="6.7265625"/>
-    <col customWidth="1" max="250" min="250" style="4" width="8"/>
-    <col customWidth="1" max="252" min="251" style="4" width="12.26953125"/>
-    <col customWidth="1" max="503" min="253" style="4" width="9.08984375"/>
-    <col customWidth="1" max="505" min="504" style="4" width="6.7265625"/>
-    <col customWidth="1" max="506" min="506" style="4" width="8"/>
-    <col customWidth="1" max="508" min="507" style="4" width="12.26953125"/>
-    <col customWidth="1" max="759" min="509" style="4" width="9.08984375"/>
-    <col customWidth="1" max="761" min="760" style="4" width="6.7265625"/>
-    <col customWidth="1" max="762" min="762" style="4" width="8"/>
-    <col customWidth="1" max="764" min="763" style="4" width="12.26953125"/>
-    <col customWidth="1" max="1015" min="765" style="4" width="9.08984375"/>
-    <col customWidth="1" max="1017" min="1016" style="4" width="6.7265625"/>
-    <col customWidth="1" max="1018" min="1018" style="4" width="8"/>
-    <col customWidth="1" max="1020" min="1019" style="4" width="12.26953125"/>
-    <col customWidth="1" max="1271" min="1021" style="4" width="9.08984375"/>
-    <col customWidth="1" max="1273" min="1272" style="4" width="6.7265625"/>
-    <col customWidth="1" max="1274" min="1274" style="4" width="8"/>
-    <col customWidth="1" max="1276" min="1275" style="4" width="12.26953125"/>
-    <col customWidth="1" max="1527" min="1277" style="4" width="9.08984375"/>
-    <col customWidth="1" max="1529" min="1528" style="4" width="6.7265625"/>
-    <col customWidth="1" max="1530" min="1530" style="4" width="8"/>
-    <col customWidth="1" max="1532" min="1531" style="4" width="12.26953125"/>
-    <col customWidth="1" max="1783" min="1533" style="4" width="9.08984375"/>
-    <col customWidth="1" max="1785" min="1784" style="4" width="6.7265625"/>
-    <col customWidth="1" max="1786" min="1786" style="4" width="8"/>
-    <col customWidth="1" max="1788" min="1787" style="4" width="12.26953125"/>
-    <col customWidth="1" max="2039" min="1789" style="4" width="9.08984375"/>
-    <col customWidth="1" max="2041" min="2040" style="4" width="6.7265625"/>
-    <col customWidth="1" max="2042" min="2042" style="4" width="8"/>
-    <col customWidth="1" max="2044" min="2043" style="4" width="12.26953125"/>
-    <col customWidth="1" max="2295" min="2045" style="4" width="9.08984375"/>
-    <col customWidth="1" max="2297" min="2296" style="4" width="6.7265625"/>
-    <col customWidth="1" max="2298" min="2298" style="4" width="8"/>
-    <col customWidth="1" max="2300" min="2299" style="4" width="12.26953125"/>
-    <col customWidth="1" max="2551" min="2301" style="4" width="9.08984375"/>
-    <col customWidth="1" max="2553" min="2552" style="4" width="6.7265625"/>
-    <col customWidth="1" max="2554" min="2554" style="4" width="8"/>
-    <col customWidth="1" max="2556" min="2555" style="4" width="12.26953125"/>
-    <col customWidth="1" max="2807" min="2557" style="4" width="9.08984375"/>
-    <col customWidth="1" max="2809" min="2808" style="4" width="6.7265625"/>
-    <col customWidth="1" max="2810" min="2810" style="4" width="8"/>
-    <col customWidth="1" max="2812" min="2811" style="4" width="12.26953125"/>
-    <col customWidth="1" max="3063" min="2813" style="4" width="9.08984375"/>
-    <col customWidth="1" max="3065" min="3064" style="4" width="6.7265625"/>
-    <col customWidth="1" max="3066" min="3066" style="4" width="8"/>
-    <col customWidth="1" max="3068" min="3067" style="4" width="12.26953125"/>
-    <col customWidth="1" max="3319" min="3069" style="4" width="9.08984375"/>
-    <col customWidth="1" max="3321" min="3320" style="4" width="6.7265625"/>
-    <col customWidth="1" max="3322" min="3322" style="4" width="8"/>
-    <col customWidth="1" max="3324" min="3323" style="4" width="12.26953125"/>
-    <col customWidth="1" max="3575" min="3325" style="4" width="9.08984375"/>
-    <col customWidth="1" max="3577" min="3576" style="4" width="6.7265625"/>
-    <col customWidth="1" max="3578" min="3578" style="4" width="8"/>
-    <col customWidth="1" max="3580" min="3579" style="4" width="12.26953125"/>
-    <col customWidth="1" max="3831" min="3581" style="4" width="9.08984375"/>
-    <col customWidth="1" max="3833" min="3832" style="4" width="6.7265625"/>
-    <col customWidth="1" max="3834" min="3834" style="4" width="8"/>
-    <col customWidth="1" max="3836" min="3835" style="4" width="12.26953125"/>
-    <col customWidth="1" max="4087" min="3837" style="4" width="9.08984375"/>
-    <col customWidth="1" max="4089" min="4088" style="4" width="6.7265625"/>
-    <col customWidth="1" max="4090" min="4090" style="4" width="8"/>
-    <col customWidth="1" max="4092" min="4091" style="4" width="12.26953125"/>
-    <col customWidth="1" max="4343" min="4093" style="4" width="9.08984375"/>
-    <col customWidth="1" max="4345" min="4344" style="4" width="6.7265625"/>
-    <col customWidth="1" max="4346" min="4346" style="4" width="8"/>
-    <col customWidth="1" max="4348" min="4347" style="4" width="12.26953125"/>
-    <col customWidth="1" max="4599" min="4349" style="4" width="9.08984375"/>
-    <col customWidth="1" max="4601" min="4600" style="4" width="6.7265625"/>
-    <col customWidth="1" max="4602" min="4602" style="4" width="8"/>
-    <col customWidth="1" max="4604" min="4603" style="4" width="12.26953125"/>
-    <col customWidth="1" max="4855" min="4605" style="4" width="9.08984375"/>
-    <col customWidth="1" max="4857" min="4856" style="4" width="6.7265625"/>
-    <col customWidth="1" max="4858" min="4858" style="4" width="8"/>
-    <col customWidth="1" max="4860" min="4859" style="4" width="12.26953125"/>
-    <col customWidth="1" max="5111" min="4861" style="4" width="9.08984375"/>
-    <col customWidth="1" max="5113" min="5112" style="4" width="6.7265625"/>
-    <col customWidth="1" max="5114" min="5114" style="4" width="8"/>
-    <col customWidth="1" max="5116" min="5115" style="4" width="12.26953125"/>
-    <col customWidth="1" max="5367" min="5117" style="4" width="9.08984375"/>
-    <col customWidth="1" max="5369" min="5368" style="4" width="6.7265625"/>
-    <col customWidth="1" max="5370" min="5370" style="4" width="8"/>
-    <col customWidth="1" max="5372" min="5371" style="4" width="12.26953125"/>
-    <col customWidth="1" max="5623" min="5373" style="4" width="9.08984375"/>
-    <col customWidth="1" max="5625" min="5624" style="4" width="6.7265625"/>
-    <col customWidth="1" max="5626" min="5626" style="4" width="8"/>
-    <col customWidth="1" max="5628" min="5627" style="4" width="12.26953125"/>
-    <col customWidth="1" max="5879" min="5629" style="4" width="9.08984375"/>
-    <col customWidth="1" max="5881" min="5880" style="4" width="6.7265625"/>
-    <col customWidth="1" max="5882" min="5882" style="4" width="8"/>
-    <col customWidth="1" max="5884" min="5883" style="4" width="12.26953125"/>
-    <col customWidth="1" max="6135" min="5885" style="4" width="9.08984375"/>
-    <col customWidth="1" max="6137" min="6136" style="4" width="6.7265625"/>
-    <col customWidth="1" max="6138" min="6138" style="4" width="8"/>
-    <col customWidth="1" max="6140" min="6139" style="4" width="12.26953125"/>
-    <col customWidth="1" max="6391" min="6141" style="4" width="9.08984375"/>
-    <col customWidth="1" max="6393" min="6392" style="4" width="6.7265625"/>
-    <col customWidth="1" max="6394" min="6394" style="4" width="8"/>
-    <col customWidth="1" max="6396" min="6395" style="4" width="12.26953125"/>
-    <col customWidth="1" max="6647" min="6397" style="4" width="9.08984375"/>
-    <col customWidth="1" max="6649" min="6648" style="4" width="6.7265625"/>
-    <col customWidth="1" max="6650" min="6650" style="4" width="8"/>
-    <col customWidth="1" max="6652" min="6651" style="4" width="12.26953125"/>
-    <col customWidth="1" max="6903" min="6653" style="4" width="9.08984375"/>
-    <col customWidth="1" max="6905" min="6904" style="4" width="6.7265625"/>
-    <col customWidth="1" max="6906" min="6906" style="4" width="8"/>
-    <col customWidth="1" max="6908" min="6907" style="4" width="12.26953125"/>
-    <col customWidth="1" max="7159" min="6909" style="4" width="9.08984375"/>
-    <col customWidth="1" max="7161" min="7160" style="4" width="6.7265625"/>
-    <col customWidth="1" max="7162" min="7162" style="4" width="8"/>
-    <col customWidth="1" max="7164" min="7163" style="4" width="12.26953125"/>
-    <col customWidth="1" max="7415" min="7165" style="4" width="9.08984375"/>
-    <col customWidth="1" max="7417" min="7416" style="4" width="6.7265625"/>
-    <col customWidth="1" max="7418" min="7418" style="4" width="8"/>
-    <col customWidth="1" max="7420" min="7419" style="4" width="12.26953125"/>
-    <col customWidth="1" max="7671" min="7421" style="4" width="9.08984375"/>
-    <col customWidth="1" max="7673" min="7672" style="4" width="6.7265625"/>
-    <col customWidth="1" max="7674" min="7674" style="4" width="8"/>
-    <col customWidth="1" max="7676" min="7675" style="4" width="12.26953125"/>
-    <col customWidth="1" max="7927" min="7677" style="4" width="9.08984375"/>
-    <col customWidth="1" max="7929" min="7928" style="4" width="6.7265625"/>
-    <col customWidth="1" max="7930" min="7930" style="4" width="8"/>
-    <col customWidth="1" max="7932" min="7931" style="4" width="12.26953125"/>
-    <col customWidth="1" max="8183" min="7933" style="4" width="9.08984375"/>
-    <col customWidth="1" max="8185" min="8184" style="4" width="6.7265625"/>
-    <col customWidth="1" max="8186" min="8186" style="4" width="8"/>
-    <col customWidth="1" max="8188" min="8187" style="4" width="12.26953125"/>
-    <col customWidth="1" max="8439" min="8189" style="4" width="9.08984375"/>
-    <col customWidth="1" max="8441" min="8440" style="4" width="6.7265625"/>
-    <col customWidth="1" max="8442" min="8442" style="4" width="8"/>
-    <col customWidth="1" max="8444" min="8443" style="4" width="12.26953125"/>
-    <col customWidth="1" max="8695" min="8445" style="4" width="9.08984375"/>
-    <col customWidth="1" max="8697" min="8696" style="4" width="6.7265625"/>
-    <col customWidth="1" max="8698" min="8698" style="4" width="8"/>
-    <col customWidth="1" max="8700" min="8699" style="4" width="12.26953125"/>
-    <col customWidth="1" max="8951" min="8701" style="4" width="9.08984375"/>
-    <col customWidth="1" max="8953" min="8952" style="4" width="6.7265625"/>
-    <col customWidth="1" max="8954" min="8954" style="4" width="8"/>
-    <col customWidth="1" max="8956" min="8955" style="4" width="12.26953125"/>
-    <col customWidth="1" max="9207" min="8957" style="4" width="9.08984375"/>
-    <col customWidth="1" max="9209" min="9208" style="4" width="6.7265625"/>
-    <col customWidth="1" max="9210" min="9210" style="4" width="8"/>
-    <col customWidth="1" max="9212" min="9211" style="4" width="12.26953125"/>
-    <col customWidth="1" max="9463" min="9213" style="4" width="9.08984375"/>
-    <col customWidth="1" max="9465" min="9464" style="4" width="6.7265625"/>
-    <col customWidth="1" max="9466" min="9466" style="4" width="8"/>
-    <col customWidth="1" max="9468" min="9467" style="4" width="12.26953125"/>
-    <col customWidth="1" max="9719" min="9469" style="4" width="9.08984375"/>
-    <col customWidth="1" max="9721" min="9720" style="4" width="6.7265625"/>
-    <col customWidth="1" max="9722" min="9722" style="4" width="8"/>
-    <col customWidth="1" max="9724" min="9723" style="4" width="12.26953125"/>
-    <col customWidth="1" max="9975" min="9725" style="4" width="9.08984375"/>
-    <col customWidth="1" max="9977" min="9976" style="4" width="6.7265625"/>
-    <col customWidth="1" max="9978" min="9978" style="4" width="8"/>
-    <col customWidth="1" max="9980" min="9979" style="4" width="12.26953125"/>
-    <col customWidth="1" max="10231" min="9981" style="4" width="9.08984375"/>
-    <col customWidth="1" max="10233" min="10232" style="4" width="6.7265625"/>
-    <col customWidth="1" max="10234" min="10234" style="4" width="8"/>
-    <col customWidth="1" max="10236" min="10235" style="4" width="12.26953125"/>
-    <col customWidth="1" max="10487" min="10237" style="4" width="9.08984375"/>
-    <col customWidth="1" max="10489" min="10488" style="4" width="6.7265625"/>
-    <col customWidth="1" max="10490" min="10490" style="4" width="8"/>
-    <col customWidth="1" max="10492" min="10491" style="4" width="12.26953125"/>
-    <col customWidth="1" max="10743" min="10493" style="4" width="9.08984375"/>
-    <col customWidth="1" max="10745" min="10744" style="4" width="6.7265625"/>
-    <col customWidth="1" max="10746" min="10746" style="4" width="8"/>
-    <col customWidth="1" max="10748" min="10747" style="4" width="12.26953125"/>
-    <col customWidth="1" max="10999" min="10749" style="4" width="9.08984375"/>
-    <col customWidth="1" max="11001" min="11000" style="4" width="6.7265625"/>
-    <col customWidth="1" max="11002" min="11002" style="4" width="8"/>
-    <col customWidth="1" max="11004" min="11003" style="4" width="12.26953125"/>
-    <col customWidth="1" max="11255" min="11005" style="4" width="9.08984375"/>
-    <col customWidth="1" max="11257" min="11256" style="4" width="6.7265625"/>
-    <col customWidth="1" max="11258" min="11258" style="4" width="8"/>
-    <col customWidth="1" max="11260" min="11259" style="4" width="12.26953125"/>
-    <col customWidth="1" max="11511" min="11261" style="4" width="9.08984375"/>
-    <col customWidth="1" max="11513" min="11512" style="4" width="6.7265625"/>
-    <col customWidth="1" max="11514" min="11514" style="4" width="8"/>
-    <col customWidth="1" max="11516" min="11515" style="4" width="12.26953125"/>
-    <col customWidth="1" max="11767" min="11517" style="4" width="9.08984375"/>
-    <col customWidth="1" max="11769" min="11768" style="4" width="6.7265625"/>
-    <col customWidth="1" max="11770" min="11770" style="4" width="8"/>
-    <col customWidth="1" max="11772" min="11771" style="4" width="12.26953125"/>
-    <col customWidth="1" max="12023" min="11773" style="4" width="9.08984375"/>
-    <col customWidth="1" max="12025" min="12024" style="4" width="6.7265625"/>
-    <col customWidth="1" max="12026" min="12026" style="4" width="8"/>
-    <col customWidth="1" max="12028" min="12027" style="4" width="12.26953125"/>
-    <col customWidth="1" max="12279" min="12029" style="4" width="9.08984375"/>
-    <col customWidth="1" max="12281" min="12280" style="4" width="6.7265625"/>
-    <col customWidth="1" max="12282" min="12282" style="4" width="8"/>
-    <col customWidth="1" max="12284" min="12283" style="4" width="12.26953125"/>
-    <col customWidth="1" max="12535" min="12285" style="4" width="9.08984375"/>
-    <col customWidth="1" max="12537" min="12536" style="4" width="6.7265625"/>
-    <col customWidth="1" max="12538" min="12538" style="4" width="8"/>
-    <col customWidth="1" max="12540" min="12539" style="4" width="12.26953125"/>
-    <col customWidth="1" max="12791" min="12541" style="4" width="9.08984375"/>
-    <col customWidth="1" max="12793" min="12792" style="4" width="6.7265625"/>
-    <col customWidth="1" max="12794" min="12794" style="4" width="8"/>
-    <col customWidth="1" max="12796" min="12795" style="4" width="12.26953125"/>
-    <col customWidth="1" max="13047" min="12797" style="4" width="9.08984375"/>
-    <col customWidth="1" max="13049" min="13048" style="4" width="6.7265625"/>
-    <col customWidth="1" max="13050" min="13050" style="4" width="8"/>
-    <col customWidth="1" max="13052" min="13051" style="4" width="12.26953125"/>
-    <col customWidth="1" max="13303" min="13053" style="4" width="9.08984375"/>
-    <col customWidth="1" max="13305" min="13304" style="4" width="6.7265625"/>
-    <col customWidth="1" max="13306" min="13306" style="4" width="8"/>
-    <col customWidth="1" max="13308" min="13307" style="4" width="12.26953125"/>
-    <col customWidth="1" max="13559" min="13309" style="4" width="9.08984375"/>
-    <col customWidth="1" max="13561" min="13560" style="4" width="6.7265625"/>
-    <col customWidth="1" max="13562" min="13562" style="4" width="8"/>
-    <col customWidth="1" max="13564" min="13563" style="4" width="12.26953125"/>
-    <col customWidth="1" max="13815" min="13565" style="4" width="9.08984375"/>
-    <col customWidth="1" max="13817" min="13816" style="4" width="6.7265625"/>
-    <col customWidth="1" max="13818" min="13818" style="4" width="8"/>
-    <col customWidth="1" max="13820" min="13819" style="4" width="12.26953125"/>
-    <col customWidth="1" max="14071" min="13821" style="4" width="9.08984375"/>
-    <col customWidth="1" max="14073" min="14072" style="4" width="6.7265625"/>
-    <col customWidth="1" max="14074" min="14074" style="4" width="8"/>
-    <col customWidth="1" max="14076" min="14075" style="4" width="12.26953125"/>
-    <col customWidth="1" max="14327" min="14077" style="4" width="9.08984375"/>
-    <col customWidth="1" max="14329" min="14328" style="4" width="6.7265625"/>
-    <col customWidth="1" max="14330" min="14330" style="4" width="8"/>
-    <col customWidth="1" max="14332" min="14331" style="4" width="12.26953125"/>
-    <col customWidth="1" max="14583" min="14333" style="4" width="9.08984375"/>
-    <col customWidth="1" max="14585" min="14584" style="4" width="6.7265625"/>
-    <col customWidth="1" max="14586" min="14586" style="4" width="8"/>
-    <col customWidth="1" max="14588" min="14587" style="4" width="12.26953125"/>
-    <col customWidth="1" max="14839" min="14589" style="4" width="9.08984375"/>
-    <col customWidth="1" max="14841" min="14840" style="4" width="6.7265625"/>
-    <col customWidth="1" max="14842" min="14842" style="4" width="8"/>
-    <col customWidth="1" max="14844" min="14843" style="4" width="12.26953125"/>
-    <col customWidth="1" max="15095" min="14845" style="4" width="9.08984375"/>
-    <col customWidth="1" max="15097" min="15096" style="4" width="6.7265625"/>
-    <col customWidth="1" max="15098" min="15098" style="4" width="8"/>
-    <col customWidth="1" max="15100" min="15099" style="4" width="12.26953125"/>
-    <col customWidth="1" max="15351" min="15101" style="4" width="9.08984375"/>
-    <col customWidth="1" max="15353" min="15352" style="4" width="6.7265625"/>
-    <col customWidth="1" max="15354" min="15354" style="4" width="8"/>
-    <col customWidth="1" max="15356" min="15355" style="4" width="12.26953125"/>
-    <col customWidth="1" max="15607" min="15357" style="4" width="9.08984375"/>
-    <col customWidth="1" max="15609" min="15608" style="4" width="6.7265625"/>
-    <col customWidth="1" max="15610" min="15610" style="4" width="8"/>
-    <col customWidth="1" max="15612" min="15611" style="4" width="12.26953125"/>
-    <col customWidth="1" max="15863" min="15613" style="4" width="9.08984375"/>
-    <col customWidth="1" max="15865" min="15864" style="4" width="6.7265625"/>
-    <col customWidth="1" max="15866" min="15866" style="4" width="8"/>
-    <col customWidth="1" max="15868" min="15867" style="4" width="12.26953125"/>
-    <col customWidth="1" max="16119" min="15869" style="4" width="9.08984375"/>
-    <col customWidth="1" max="16121" min="16120" style="4" width="6.7265625"/>
-    <col customWidth="1" max="16122" min="16122" style="4" width="8"/>
-    <col customWidth="1" max="16124" min="16123" style="4" width="12.26953125"/>
-    <col customWidth="1" max="16384" min="16125" style="4" width="9.08984375"/>
+    <col width="6.7265625" customWidth="1" style="4" min="1" max="1"/>
+    <col width="9.6328125" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
+    <col width="26.7265625" bestFit="1" customWidth="1" style="4" min="3" max="3"/>
+    <col width="8.7265625" customWidth="1" style="4" min="4" max="4"/>
+    <col width="9.6328125" bestFit="1" customWidth="1" style="4" min="5" max="5"/>
+    <col width="10.6328125" customWidth="1" style="4" min="6" max="13"/>
+    <col width="9.08984375" customWidth="1" style="4" min="14" max="247"/>
+    <col width="6.7265625" customWidth="1" style="4" min="248" max="249"/>
+    <col width="8" customWidth="1" style="4" min="250" max="250"/>
+    <col width="12.26953125" customWidth="1" style="4" min="251" max="252"/>
+    <col width="9.08984375" customWidth="1" style="4" min="253" max="503"/>
+    <col width="6.7265625" customWidth="1" style="4" min="504" max="505"/>
+    <col width="8" customWidth="1" style="4" min="506" max="506"/>
+    <col width="12.26953125" customWidth="1" style="4" min="507" max="508"/>
+    <col width="9.08984375" customWidth="1" style="4" min="509" max="759"/>
+    <col width="6.7265625" customWidth="1" style="4" min="760" max="761"/>
+    <col width="8" customWidth="1" style="4" min="762" max="762"/>
+    <col width="12.26953125" customWidth="1" style="4" min="763" max="764"/>
+    <col width="9.08984375" customWidth="1" style="4" min="765" max="1015"/>
+    <col width="6.7265625" customWidth="1" style="4" min="1016" max="1017"/>
+    <col width="8" customWidth="1" style="4" min="1018" max="1018"/>
+    <col width="12.26953125" customWidth="1" style="4" min="1019" max="1020"/>
+    <col width="9.08984375" customWidth="1" style="4" min="1021" max="1271"/>
+    <col width="6.7265625" customWidth="1" style="4" min="1272" max="1273"/>
+    <col width="8" customWidth="1" style="4" min="1274" max="1274"/>
+    <col width="12.26953125" customWidth="1" style="4" min="1275" max="1276"/>
+    <col width="9.08984375" customWidth="1" style="4" min="1277" max="1527"/>
+    <col width="6.7265625" customWidth="1" style="4" min="1528" max="1529"/>
+    <col width="8" customWidth="1" style="4" min="1530" max="1530"/>
+    <col width="12.26953125" customWidth="1" style="4" min="1531" max="1532"/>
+    <col width="9.08984375" customWidth="1" style="4" min="1533" max="1783"/>
+    <col width="6.7265625" customWidth="1" style="4" min="1784" max="1785"/>
+    <col width="8" customWidth="1" style="4" min="1786" max="1786"/>
+    <col width="12.26953125" customWidth="1" style="4" min="1787" max="1788"/>
+    <col width="9.08984375" customWidth="1" style="4" min="1789" max="2039"/>
+    <col width="6.7265625" customWidth="1" style="4" min="2040" max="2041"/>
+    <col width="8" customWidth="1" style="4" min="2042" max="2042"/>
+    <col width="12.26953125" customWidth="1" style="4" min="2043" max="2044"/>
+    <col width="9.08984375" customWidth="1" style="4" min="2045" max="2295"/>
+    <col width="6.7265625" customWidth="1" style="4" min="2296" max="2297"/>
+    <col width="8" customWidth="1" style="4" min="2298" max="2298"/>
+    <col width="12.26953125" customWidth="1" style="4" min="2299" max="2300"/>
+    <col width="9.08984375" customWidth="1" style="4" min="2301" max="2551"/>
+    <col width="6.7265625" customWidth="1" style="4" min="2552" max="2553"/>
+    <col width="8" customWidth="1" style="4" min="2554" max="2554"/>
+    <col width="12.26953125" customWidth="1" style="4" min="2555" max="2556"/>
+    <col width="9.08984375" customWidth="1" style="4" min="2557" max="2807"/>
+    <col width="6.7265625" customWidth="1" style="4" min="2808" max="2809"/>
+    <col width="8" customWidth="1" style="4" min="2810" max="2810"/>
+    <col width="12.26953125" customWidth="1" style="4" min="2811" max="2812"/>
+    <col width="9.08984375" customWidth="1" style="4" min="2813" max="3063"/>
+    <col width="6.7265625" customWidth="1" style="4" min="3064" max="3065"/>
+    <col width="8" customWidth="1" style="4" min="3066" max="3066"/>
+    <col width="12.26953125" customWidth="1" style="4" min="3067" max="3068"/>
+    <col width="9.08984375" customWidth="1" style="4" min="3069" max="3319"/>
+    <col width="6.7265625" customWidth="1" style="4" min="3320" max="3321"/>
+    <col width="8" customWidth="1" style="4" min="3322" max="3322"/>
+    <col width="12.26953125" customWidth="1" style="4" min="3323" max="3324"/>
+    <col width="9.08984375" customWidth="1" style="4" min="3325" max="3575"/>
+    <col width="6.7265625" customWidth="1" style="4" min="3576" max="3577"/>
+    <col width="8" customWidth="1" style="4" min="3578" max="3578"/>
+    <col width="12.26953125" customWidth="1" style="4" min="3579" max="3580"/>
+    <col width="9.08984375" customWidth="1" style="4" min="3581" max="3831"/>
+    <col width="6.7265625" customWidth="1" style="4" min="3832" max="3833"/>
+    <col width="8" customWidth="1" style="4" min="3834" max="3834"/>
+    <col width="12.26953125" customWidth="1" style="4" min="3835" max="3836"/>
+    <col width="9.08984375" customWidth="1" style="4" min="3837" max="4087"/>
+    <col width="6.7265625" customWidth="1" style="4" min="4088" max="4089"/>
+    <col width="8" customWidth="1" style="4" min="4090" max="4090"/>
+    <col width="12.26953125" customWidth="1" style="4" min="4091" max="4092"/>
+    <col width="9.08984375" customWidth="1" style="4" min="4093" max="4343"/>
+    <col width="6.7265625" customWidth="1" style="4" min="4344" max="4345"/>
+    <col width="8" customWidth="1" style="4" min="4346" max="4346"/>
+    <col width="12.26953125" customWidth="1" style="4" min="4347" max="4348"/>
+    <col width="9.08984375" customWidth="1" style="4" min="4349" max="4599"/>
+    <col width="6.7265625" customWidth="1" style="4" min="4600" max="4601"/>
+    <col width="8" customWidth="1" style="4" min="4602" max="4602"/>
+    <col width="12.26953125" customWidth="1" style="4" min="4603" max="4604"/>
+    <col width="9.08984375" customWidth="1" style="4" min="4605" max="4855"/>
+    <col width="6.7265625" customWidth="1" style="4" min="4856" max="4857"/>
+    <col width="8" customWidth="1" style="4" min="4858" max="4858"/>
+    <col width="12.26953125" customWidth="1" style="4" min="4859" max="4860"/>
+    <col width="9.08984375" customWidth="1" style="4" min="4861" max="5111"/>
+    <col width="6.7265625" customWidth="1" style="4" min="5112" max="5113"/>
+    <col width="8" customWidth="1" style="4" min="5114" max="5114"/>
+    <col width="12.26953125" customWidth="1" style="4" min="5115" max="5116"/>
+    <col width="9.08984375" customWidth="1" style="4" min="5117" max="5367"/>
+    <col width="6.7265625" customWidth="1" style="4" min="5368" max="5369"/>
+    <col width="8" customWidth="1" style="4" min="5370" max="5370"/>
+    <col width="12.26953125" customWidth="1" style="4" min="5371" max="5372"/>
+    <col width="9.08984375" customWidth="1" style="4" min="5373" max="5623"/>
+    <col width="6.7265625" customWidth="1" style="4" min="5624" max="5625"/>
+    <col width="8" customWidth="1" style="4" min="5626" max="5626"/>
+    <col width="12.26953125" customWidth="1" style="4" min="5627" max="5628"/>
+    <col width="9.08984375" customWidth="1" style="4" min="5629" max="5879"/>
+    <col width="6.7265625" customWidth="1" style="4" min="5880" max="5881"/>
+    <col width="8" customWidth="1" style="4" min="5882" max="5882"/>
+    <col width="12.26953125" customWidth="1" style="4" min="5883" max="5884"/>
+    <col width="9.08984375" customWidth="1" style="4" min="5885" max="6135"/>
+    <col width="6.7265625" customWidth="1" style="4" min="6136" max="6137"/>
+    <col width="8" customWidth="1" style="4" min="6138" max="6138"/>
+    <col width="12.26953125" customWidth="1" style="4" min="6139" max="6140"/>
+    <col width="9.08984375" customWidth="1" style="4" min="6141" max="6391"/>
+    <col width="6.7265625" customWidth="1" style="4" min="6392" max="6393"/>
+    <col width="8" customWidth="1" style="4" min="6394" max="6394"/>
+    <col width="12.26953125" customWidth="1" style="4" min="6395" max="6396"/>
+    <col width="9.08984375" customWidth="1" style="4" min="6397" max="6647"/>
+    <col width="6.7265625" customWidth="1" style="4" min="6648" max="6649"/>
+    <col width="8" customWidth="1" style="4" min="6650" max="6650"/>
+    <col width="12.26953125" customWidth="1" style="4" min="6651" max="6652"/>
+    <col width="9.08984375" customWidth="1" style="4" min="6653" max="6903"/>
+    <col width="6.7265625" customWidth="1" style="4" min="6904" max="6905"/>
+    <col width="8" customWidth="1" style="4" min="6906" max="6906"/>
+    <col width="12.26953125" customWidth="1" style="4" min="6907" max="6908"/>
+    <col width="9.08984375" customWidth="1" style="4" min="6909" max="7159"/>
+    <col width="6.7265625" customWidth="1" style="4" min="7160" max="7161"/>
+    <col width="8" customWidth="1" style="4" min="7162" max="7162"/>
+    <col width="12.26953125" customWidth="1" style="4" min="7163" max="7164"/>
+    <col width="9.08984375" customWidth="1" style="4" min="7165" max="7415"/>
+    <col width="6.7265625" customWidth="1" style="4" min="7416" max="7417"/>
+    <col width="8" customWidth="1" style="4" min="7418" max="7418"/>
+    <col width="12.26953125" customWidth="1" style="4" min="7419" max="7420"/>
+    <col width="9.08984375" customWidth="1" style="4" min="7421" max="7671"/>
+    <col width="6.7265625" customWidth="1" style="4" min="7672" max="7673"/>
+    <col width="8" customWidth="1" style="4" min="7674" max="7674"/>
+    <col width="12.26953125" customWidth="1" style="4" min="7675" max="7676"/>
+    <col width="9.08984375" customWidth="1" style="4" min="7677" max="7927"/>
+    <col width="6.7265625" customWidth="1" style="4" min="7928" max="7929"/>
+    <col width="8" customWidth="1" style="4" min="7930" max="7930"/>
+    <col width="12.26953125" customWidth="1" style="4" min="7931" max="7932"/>
+    <col width="9.08984375" customWidth="1" style="4" min="7933" max="8183"/>
+    <col width="6.7265625" customWidth="1" style="4" min="8184" max="8185"/>
+    <col width="8" customWidth="1" style="4" min="8186" max="8186"/>
+    <col width="12.26953125" customWidth="1" style="4" min="8187" max="8188"/>
+    <col width="9.08984375" customWidth="1" style="4" min="8189" max="8439"/>
+    <col width="6.7265625" customWidth="1" style="4" min="8440" max="8441"/>
+    <col width="8" customWidth="1" style="4" min="8442" max="8442"/>
+    <col width="12.26953125" customWidth="1" style="4" min="8443" max="8444"/>
+    <col width="9.08984375" customWidth="1" style="4" min="8445" max="8695"/>
+    <col width="6.7265625" customWidth="1" style="4" min="8696" max="8697"/>
+    <col width="8" customWidth="1" style="4" min="8698" max="8698"/>
+    <col width="12.26953125" customWidth="1" style="4" min="8699" max="8700"/>
+    <col width="9.08984375" customWidth="1" style="4" min="8701" max="8951"/>
+    <col width="6.7265625" customWidth="1" style="4" min="8952" max="8953"/>
+    <col width="8" customWidth="1" style="4" min="8954" max="8954"/>
+    <col width="12.26953125" customWidth="1" style="4" min="8955" max="8956"/>
+    <col width="9.08984375" customWidth="1" style="4" min="8957" max="9207"/>
+    <col width="6.7265625" customWidth="1" style="4" min="9208" max="9209"/>
+    <col width="8" customWidth="1" style="4" min="9210" max="9210"/>
+    <col width="12.26953125" customWidth="1" style="4" min="9211" max="9212"/>
+    <col width="9.08984375" customWidth="1" style="4" min="9213" max="9463"/>
+    <col width="6.7265625" customWidth="1" style="4" min="9464" max="9465"/>
+    <col width="8" customWidth="1" style="4" min="9466" max="9466"/>
+    <col width="12.26953125" customWidth="1" style="4" min="9467" max="9468"/>
+    <col width="9.08984375" customWidth="1" style="4" min="9469" max="9719"/>
+    <col width="6.7265625" customWidth="1" style="4" min="9720" max="9721"/>
+    <col width="8" customWidth="1" style="4" min="9722" max="9722"/>
+    <col width="12.26953125" customWidth="1" style="4" min="9723" max="9724"/>
+    <col width="9.08984375" customWidth="1" style="4" min="9725" max="9975"/>
+    <col width="6.7265625" customWidth="1" style="4" min="9976" max="9977"/>
+    <col width="8" customWidth="1" style="4" min="9978" max="9978"/>
+    <col width="12.26953125" customWidth="1" style="4" min="9979" max="9980"/>
+    <col width="9.08984375" customWidth="1" style="4" min="9981" max="10231"/>
+    <col width="6.7265625" customWidth="1" style="4" min="10232" max="10233"/>
+    <col width="8" customWidth="1" style="4" min="10234" max="10234"/>
+    <col width="12.26953125" customWidth="1" style="4" min="10235" max="10236"/>
+    <col width="9.08984375" customWidth="1" style="4" min="10237" max="10487"/>
+    <col width="6.7265625" customWidth="1" style="4" min="10488" max="10489"/>
+    <col width="8" customWidth="1" style="4" min="10490" max="10490"/>
+    <col width="12.26953125" customWidth="1" style="4" min="10491" max="10492"/>
+    <col width="9.08984375" customWidth="1" style="4" min="10493" max="10743"/>
+    <col width="6.7265625" customWidth="1" style="4" min="10744" max="10745"/>
+    <col width="8" customWidth="1" style="4" min="10746" max="10746"/>
+    <col width="12.26953125" customWidth="1" style="4" min="10747" max="10748"/>
+    <col width="9.08984375" customWidth="1" style="4" min="10749" max="10999"/>
+    <col width="6.7265625" customWidth="1" style="4" min="11000" max="11001"/>
+    <col width="8" customWidth="1" style="4" min="11002" max="11002"/>
+    <col width="12.26953125" customWidth="1" style="4" min="11003" max="11004"/>
+    <col width="9.08984375" customWidth="1" style="4" min="11005" max="11255"/>
+    <col width="6.7265625" customWidth="1" style="4" min="11256" max="11257"/>
+    <col width="8" customWidth="1" style="4" min="11258" max="11258"/>
+    <col width="12.26953125" customWidth="1" style="4" min="11259" max="11260"/>
+    <col width="9.08984375" customWidth="1" style="4" min="11261" max="11511"/>
+    <col width="6.7265625" customWidth="1" style="4" min="11512" max="11513"/>
+    <col width="8" customWidth="1" style="4" min="11514" max="11514"/>
+    <col width="12.26953125" customWidth="1" style="4" min="11515" max="11516"/>
+    <col width="9.08984375" customWidth="1" style="4" min="11517" max="11767"/>
+    <col width="6.7265625" customWidth="1" style="4" min="11768" max="11769"/>
+    <col width="8" customWidth="1" style="4" min="11770" max="11770"/>
+    <col width="12.26953125" customWidth="1" style="4" min="11771" max="11772"/>
+    <col width="9.08984375" customWidth="1" style="4" min="11773" max="12023"/>
+    <col width="6.7265625" customWidth="1" style="4" min="12024" max="12025"/>
+    <col width="8" customWidth="1" style="4" min="12026" max="12026"/>
+    <col width="12.26953125" customWidth="1" style="4" min="12027" max="12028"/>
+    <col width="9.08984375" customWidth="1" style="4" min="12029" max="12279"/>
+    <col width="6.7265625" customWidth="1" style="4" min="12280" max="12281"/>
+    <col width="8" customWidth="1" style="4" min="12282" max="12282"/>
+    <col width="12.26953125" customWidth="1" style="4" min="12283" max="12284"/>
+    <col width="9.08984375" customWidth="1" style="4" min="12285" max="12535"/>
+    <col width="6.7265625" customWidth="1" style="4" min="12536" max="12537"/>
+    <col width="8" customWidth="1" style="4" min="12538" max="12538"/>
+    <col width="12.26953125" customWidth="1" style="4" min="12539" max="12540"/>
+    <col width="9.08984375" customWidth="1" style="4" min="12541" max="12791"/>
+    <col width="6.7265625" customWidth="1" style="4" min="12792" max="12793"/>
+    <col width="8" customWidth="1" style="4" min="12794" max="12794"/>
+    <col width="12.26953125" customWidth="1" style="4" min="12795" max="12796"/>
+    <col width="9.08984375" customWidth="1" style="4" min="12797" max="13047"/>
+    <col width="6.7265625" customWidth="1" style="4" min="13048" max="13049"/>
+    <col width="8" customWidth="1" style="4" min="13050" max="13050"/>
+    <col width="12.26953125" customWidth="1" style="4" min="13051" max="13052"/>
+    <col width="9.08984375" customWidth="1" style="4" min="13053" max="13303"/>
+    <col width="6.7265625" customWidth="1" style="4" min="13304" max="13305"/>
+    <col width="8" customWidth="1" style="4" min="13306" max="13306"/>
+    <col width="12.26953125" customWidth="1" style="4" min="13307" max="13308"/>
+    <col width="9.08984375" customWidth="1" style="4" min="13309" max="13559"/>
+    <col width="6.7265625" customWidth="1" style="4" min="13560" max="13561"/>
+    <col width="8" customWidth="1" style="4" min="13562" max="13562"/>
+    <col width="12.26953125" customWidth="1" style="4" min="13563" max="13564"/>
+    <col width="9.08984375" customWidth="1" style="4" min="13565" max="13815"/>
+    <col width="6.7265625" customWidth="1" style="4" min="13816" max="13817"/>
+    <col width="8" customWidth="1" style="4" min="13818" max="13818"/>
+    <col width="12.26953125" customWidth="1" style="4" min="13819" max="13820"/>
+    <col width="9.08984375" customWidth="1" style="4" min="13821" max="14071"/>
+    <col width="6.7265625" customWidth="1" style="4" min="14072" max="14073"/>
+    <col width="8" customWidth="1" style="4" min="14074" max="14074"/>
+    <col width="12.26953125" customWidth="1" style="4" min="14075" max="14076"/>
+    <col width="9.08984375" customWidth="1" style="4" min="14077" max="14327"/>
+    <col width="6.7265625" customWidth="1" style="4" min="14328" max="14329"/>
+    <col width="8" customWidth="1" style="4" min="14330" max="14330"/>
+    <col width="12.26953125" customWidth="1" style="4" min="14331" max="14332"/>
+    <col width="9.08984375" customWidth="1" style="4" min="14333" max="14583"/>
+    <col width="6.7265625" customWidth="1" style="4" min="14584" max="14585"/>
+    <col width="8" customWidth="1" style="4" min="14586" max="14586"/>
+    <col width="12.26953125" customWidth="1" style="4" min="14587" max="14588"/>
+    <col width="9.08984375" customWidth="1" style="4" min="14589" max="14839"/>
+    <col width="6.7265625" customWidth="1" style="4" min="14840" max="14841"/>
+    <col width="8" customWidth="1" style="4" min="14842" max="14842"/>
+    <col width="12.26953125" customWidth="1" style="4" min="14843" max="14844"/>
+    <col width="9.08984375" customWidth="1" style="4" min="14845" max="15095"/>
+    <col width="6.7265625" customWidth="1" style="4" min="15096" max="15097"/>
+    <col width="8" customWidth="1" style="4" min="15098" max="15098"/>
+    <col width="12.26953125" customWidth="1" style="4" min="15099" max="15100"/>
+    <col width="9.08984375" customWidth="1" style="4" min="15101" max="15351"/>
+    <col width="6.7265625" customWidth="1" style="4" min="15352" max="15353"/>
+    <col width="8" customWidth="1" style="4" min="15354" max="15354"/>
+    <col width="12.26953125" customWidth="1" style="4" min="15355" max="15356"/>
+    <col width="9.08984375" customWidth="1" style="4" min="15357" max="15607"/>
+    <col width="6.7265625" customWidth="1" style="4" min="15608" max="15609"/>
+    <col width="8" customWidth="1" style="4" min="15610" max="15610"/>
+    <col width="12.26953125" customWidth="1" style="4" min="15611" max="15612"/>
+    <col width="9.08984375" customWidth="1" style="4" min="15613" max="15863"/>
+    <col width="6.7265625" customWidth="1" style="4" min="15864" max="15865"/>
+    <col width="8" customWidth="1" style="4" min="15866" max="15866"/>
+    <col width="12.26953125" customWidth="1" style="4" min="15867" max="15868"/>
+    <col width="9.08984375" customWidth="1" style="4" min="15869" max="16119"/>
+    <col width="6.7265625" customWidth="1" style="4" min="16120" max="16121"/>
+    <col width="8" customWidth="1" style="4" min="16122" max="16122"/>
+    <col width="12.26953125" customWidth="1" style="4" min="16123" max="16124"/>
+    <col width="9.08984375" customWidth="1" style="4" min="16125" max="16384"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="13" r="1" s="36">
+    <row r="1" ht="13" customHeight="1" s="36">
       <c r="E1" s="5" t="n"/>
     </row>
-    <row customHeight="1" ht="14" r="2" s="36">
+    <row r="2" ht="14" customHeight="1" s="36">
       <c r="E2" s="1" t="n"/>
     </row>
-    <row customHeight="1" ht="14" r="3" s="36">
+    <row r="3" ht="14" customHeight="1" s="36">
       <c r="E3" s="1" t="n"/>
     </row>
     <row r="4">
@@ -19604,7 +19604,7 @@
     <mergeCell ref="N5:O5"/>
     <mergeCell ref="P5:Q5"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" scale="98"/>
 </worksheet>
 </file>
@@ -19617,44 +19617,44 @@
   </sheetPr>
   <dimension ref="B6:V22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="11.36328125"/>
-    <col customWidth="1" max="2" min="2" style="1" width="10.36328125"/>
-    <col customWidth="1" max="3" min="3" style="1" width="9.36328125"/>
-    <col customWidth="1" max="4" min="4" style="1" width="7.453125"/>
-    <col bestFit="1" customWidth="1" max="6" min="5" style="1" width="11.36328125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="1" width="8.81640625"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="1" width="9.90625"/>
-    <col bestFit="1" customWidth="1" max="10" min="9" style="1" width="12.7265625"/>
-    <col bestFit="1" customWidth="1" max="12" min="11" style="1" width="11.36328125"/>
-    <col customWidth="1" max="14" min="13" style="1" width="11.81640625"/>
-    <col bestFit="1" customWidth="1" max="16" min="15" style="1" width="11.453125"/>
-    <col bestFit="1" customWidth="1" max="17" min="17" style="1" width="10.36328125"/>
-    <col customWidth="1" max="18" min="18" style="1" width="11"/>
-    <col customWidth="1" max="22" min="19" style="1" width="7.36328125"/>
-    <col customWidth="1" max="32" min="23" style="1" width="9"/>
-    <col bestFit="1" customWidth="1" max="33" min="33" style="1" width="5.90625"/>
-    <col bestFit="1" customWidth="1" max="34" min="34" style="1" width="7.6328125"/>
-    <col customWidth="1" max="40" min="35" style="1" width="9"/>
-    <col bestFit="1" customWidth="1" max="41" min="41" style="1" width="6.90625"/>
-    <col bestFit="1" customWidth="1" max="42" min="42" style="1" width="6.6328125"/>
-    <col bestFit="1" customWidth="1" max="43" min="43" style="1" width="4.90625"/>
-    <col bestFit="1" customWidth="1" max="44" min="44" style="1" width="4.453125"/>
-    <col bestFit="1" customWidth="1" max="45" min="45" style="1" width="4.90625"/>
-    <col bestFit="1" customWidth="1" max="46" min="46" style="1" width="4.453125"/>
-    <col customWidth="1" max="47" min="47" style="1" width="9"/>
-    <col customWidth="1" max="16384" min="48" style="1" width="9"/>
+    <col width="11.36328125" customWidth="1" style="1" min="1" max="1"/>
+    <col width="10.36328125" customWidth="1" style="1" min="2" max="2"/>
+    <col width="9.36328125" customWidth="1" style="1" min="3" max="3"/>
+    <col width="7.453125" customWidth="1" style="1" min="4" max="4"/>
+    <col width="11.36328125" bestFit="1" customWidth="1" style="1" min="5" max="6"/>
+    <col width="8.81640625" bestFit="1" customWidth="1" style="1" min="7" max="7"/>
+    <col width="9.90625" bestFit="1" customWidth="1" style="1" min="8" max="8"/>
+    <col width="12.7265625" bestFit="1" customWidth="1" style="1" min="9" max="10"/>
+    <col width="11.36328125" bestFit="1" customWidth="1" style="1" min="11" max="12"/>
+    <col width="11.81640625" customWidth="1" style="1" min="13" max="14"/>
+    <col width="11.453125" bestFit="1" customWidth="1" style="1" min="15" max="16"/>
+    <col width="10.36328125" bestFit="1" customWidth="1" style="1" min="17" max="17"/>
+    <col width="11" customWidth="1" style="1" min="18" max="18"/>
+    <col width="7.36328125" customWidth="1" style="1" min="19" max="22"/>
+    <col width="9" customWidth="1" style="1" min="23" max="32"/>
+    <col width="5.90625" bestFit="1" customWidth="1" style="1" min="33" max="33"/>
+    <col width="7.6328125" bestFit="1" customWidth="1" style="1" min="34" max="34"/>
+    <col width="9" customWidth="1" style="1" min="35" max="40"/>
+    <col width="6.90625" bestFit="1" customWidth="1" style="1" min="41" max="41"/>
+    <col width="6.6328125" bestFit="1" customWidth="1" style="1" min="42" max="42"/>
+    <col width="4.90625" bestFit="1" customWidth="1" style="1" min="43" max="43"/>
+    <col width="4.453125" bestFit="1" customWidth="1" style="1" min="44" max="44"/>
+    <col width="4.90625" bestFit="1" customWidth="1" style="1" min="45" max="45"/>
+    <col width="4.453125" bestFit="1" customWidth="1" style="1" min="46" max="46"/>
+    <col width="9" customWidth="1" style="1" min="47" max="47"/>
+    <col width="9" customWidth="1" style="1" min="48" max="16384"/>
   </cols>
   <sheetData>
     <row r="6">
       <c r="D6" s="10" t="n"/>
     </row>
-    <row customHeight="1" ht="33" r="7" s="36">
+    <row r="7" ht="33" customHeight="1" s="36">
       <c r="B7" s="11" t="inlineStr">
         <is>
           <t>Product</t>
@@ -20307,8 +20307,8 @@
       <c r="V22" s="16" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -20320,29 +20320,29 @@
   </sheetPr>
   <dimension ref="B2:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="12.5"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="18" width="5.6328125"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="18" width="5"/>
-    <col customWidth="1" max="3" min="3" style="18" width="11.6328125"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="18" width="17.08984375"/>
-    <col customWidth="1" max="5" min="5" style="18" width="6.26953125"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="18" width="4.7265625"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="18" width="13.6328125"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="18" width="16.90625"/>
-    <col customWidth="1" max="9" min="9" style="18" width="9"/>
-    <col customWidth="1" max="16384" min="10" style="18" width="9"/>
+    <col width="5.6328125" customWidth="1" style="18" min="1" max="1"/>
+    <col width="5" bestFit="1" customWidth="1" style="18" min="2" max="2"/>
+    <col width="11.6328125" customWidth="1" style="18" min="3" max="3"/>
+    <col width="17.08984375" bestFit="1" customWidth="1" style="18" min="4" max="4"/>
+    <col width="6.26953125" customWidth="1" style="18" min="5" max="5"/>
+    <col width="4.7265625" bestFit="1" customWidth="1" style="18" min="6" max="6"/>
+    <col width="13.6328125" bestFit="1" customWidth="1" style="18" min="7" max="7"/>
+    <col width="16.90625" bestFit="1" customWidth="1" style="18" min="8" max="8"/>
+    <col width="9" customWidth="1" style="18" min="9" max="9"/>
+    <col width="9" customWidth="1" style="18" min="10" max="16384"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="14" r="2" s="36">
+    <row r="2" ht="14" customHeight="1" s="36">
       <c r="C2" s="1" t="n"/>
       <c r="G2" s="1" t="n"/>
     </row>
-    <row customHeight="1" ht="14" r="3" s="36">
+    <row r="3" ht="14" customHeight="1" s="36">
       <c r="C3" s="1" t="n"/>
       <c r="G3" s="1" t="n"/>
     </row>
@@ -20424,8 +20424,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -20437,34 +20437,34 @@
   </sheetPr>
   <dimension ref="B6:T17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="1" width="10.7265625"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="1" width="11.7265625"/>
-    <col customWidth="1" max="3" min="3" style="1" width="10.26953125"/>
-    <col customWidth="1" max="4" min="4" style="1" width="9"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="1" width="10.1796875"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="1" width="12.08984375"/>
-    <col customWidth="1" max="7" min="7" style="1" width="13.7265625"/>
-    <col customWidth="1" max="9" min="8" style="1" width="9"/>
-    <col customWidth="1" max="12" min="10" style="1" width="15.81640625"/>
-    <col customWidth="1" max="16" min="13" style="1" width="10"/>
-    <col customWidth="1" max="17" min="17" style="1" width="10.6328125"/>
-    <col customWidth="1" max="18" min="18" style="1" width="11.7265625"/>
-    <col customWidth="1" max="19" min="19" style="1" width="10"/>
-    <col bestFit="1" customWidth="1" max="20" min="20" style="1" width="9"/>
-    <col customWidth="1" max="21" min="21" style="1" width="9"/>
-    <col customWidth="1" max="16384" min="22" style="1" width="9"/>
+    <col width="10.7265625" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="11.7265625" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="10.26953125" customWidth="1" style="1" min="3" max="3"/>
+    <col width="9" customWidth="1" style="1" min="4" max="4"/>
+    <col width="10.1796875" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
+    <col width="12.08984375" bestFit="1" customWidth="1" style="1" min="6" max="6"/>
+    <col width="13.7265625" customWidth="1" style="1" min="7" max="7"/>
+    <col width="9" customWidth="1" style="1" min="8" max="9"/>
+    <col width="15.81640625" customWidth="1" style="1" min="10" max="12"/>
+    <col width="10" customWidth="1" style="1" min="13" max="16"/>
+    <col width="10.6328125" customWidth="1" style="1" min="17" max="17"/>
+    <col width="11.7265625" customWidth="1" style="1" min="18" max="18"/>
+    <col width="10" customWidth="1" style="1" min="19" max="19"/>
+    <col width="9" bestFit="1" customWidth="1" style="1" min="20" max="20"/>
+    <col width="9" customWidth="1" style="1" min="21" max="21"/>
+    <col width="9" customWidth="1" style="1" min="22" max="16384"/>
   </cols>
   <sheetData>
     <row r="6">
       <c r="C6" s="10" t="n"/>
     </row>
-    <row customHeight="1" ht="28" r="7" s="36">
+    <row r="7" ht="28" customHeight="1" s="36">
       <c r="B7" s="11" t="inlineStr">
         <is>
           <t>Product</t>
@@ -20910,8 +20910,8 @@
       <c r="T17" s="16" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -20923,17 +20923,17 @@
   </sheetPr>
   <dimension ref="B5:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="9"/>
-    <col customWidth="1" max="2" min="2" style="1" width="8"/>
-    <col customWidth="1" max="10" min="3" style="1" width="14.26953125"/>
-    <col customWidth="1" max="11" min="11" style="1" width="9"/>
-    <col customWidth="1" max="16384" min="12" style="1" width="9"/>
+    <col width="9" customWidth="1" style="1" min="1" max="1"/>
+    <col width="8" customWidth="1" style="1" min="2" max="2"/>
+    <col width="14.26953125" customWidth="1" style="1" min="3" max="10"/>
+    <col width="9" customWidth="1" style="1" min="11" max="11"/>
+    <col width="9" customWidth="1" style="1" min="12" max="16384"/>
   </cols>
   <sheetData>
     <row r="5">
@@ -21590,8 +21590,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -21609,11 +21609,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="1" width="7.7265625"/>
-    <col customWidth="1" max="2" min="2" style="1" width="8.1796875"/>
-    <col customWidth="1" max="3" min="3" style="1" width="10.6328125"/>
-    <col customWidth="1" max="4" min="4" style="1" width="9"/>
-    <col customWidth="1" max="16384" min="5" style="1" width="9"/>
+    <col width="7.7265625" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="8.1796875" customWidth="1" style="1" min="2" max="2"/>
+    <col width="10.6328125" customWidth="1" style="1" min="3" max="3"/>
+    <col width="9" customWidth="1" style="1" min="4" max="4"/>
+    <col width="9" customWidth="1" style="1" min="5" max="16384"/>
   </cols>
   <sheetData>
     <row r="3">
@@ -42777,7 +42777,7 @@
       <c r="F1513" s="0" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>